<commit_message>
Adding error logs and R scripts
</commit_message>
<xml_diff>
--- a/2024PlotFFIkey.xlsx
+++ b/2024PlotFFIkey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/cfossum_nps_gov1/Documents/Desktop/FFI-QAQC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="324" documentId="8_{BAEF1074-D8DA-449E-8E21-394D9EA59B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69EDE0CA-FBD2-4333-BC8E-43FEAD9F8418}"/>
+  <xr:revisionPtr revIDLastSave="371" documentId="8_{BAEF1074-D8DA-449E-8E21-394D9EA59B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E57AA256-91F6-44EC-8242-C2ABE4995B3C}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="405" windowWidth="26085" windowHeight="14325" firstSheet="1" activeTab="4" xr2:uid="{417E2F83-A8CD-4C79-8300-D44382CA5B9F}"/>
+    <workbookView xWindow="2325" yWindow="1035" windowWidth="26430" windowHeight="14535" firstSheet="3" activeTab="6" xr2:uid="{417E2F83-A8CD-4C79-8300-D44382CA5B9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Plot Overview" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,10 @@
     <sheet name="2024 RAP Plot Queries" sheetId="5" r:id="rId3"/>
     <sheet name="2024 Allenspark Plot Queries" sheetId="6" r:id="rId4"/>
     <sheet name="FMH PIPO Plot Queries" sheetId="7" r:id="rId5"/>
-    <sheet name="RAP Protocol" sheetId="2" r:id="rId6"/>
-    <sheet name="Allenspark Protocol" sheetId="3" r:id="rId7"/>
+    <sheet name="FMH FARTR Plot Queries" sheetId="8" r:id="rId6"/>
+    <sheet name="DINO" sheetId="9" r:id="rId7"/>
+    <sheet name="RAP Protocol" sheetId="2" r:id="rId8"/>
+    <sheet name="Allenspark Protocol" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="234">
   <si>
     <t>Project Unit</t>
   </si>
@@ -572,9 +574,6 @@
     <t>Status = L</t>
   </si>
   <si>
-    <t>Height = 1, 2, 3, 4, 5, 6, or 7</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Outliers detected with Rosner's statistical test ('EnvStats' R package) </t>
   </si>
   <si>
@@ -717,6 +716,36 @@
   </si>
   <si>
     <t>Quad area = 250m</t>
+  </si>
+  <si>
+    <t>Height = 0.15, 0.3, 0.6, 1. 2, 3, 4</t>
+  </si>
+  <si>
+    <t>Reasonable BS values ( 0-5 and flagged 1 since high severity burn is uncommon)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height = 0.15, 0.3, 0.6, 1, 2, 3, 4 </t>
+  </si>
+  <si>
+    <t>Error check queries for FMH FARTR Plots</t>
+  </si>
+  <si>
+    <t>DINO Plots</t>
+  </si>
+  <si>
+    <t>Transect length = 100</t>
+  </si>
+  <si>
+    <t>Points per transect = 200</t>
+  </si>
+  <si>
+    <t>Offset = 0</t>
+  </si>
+  <si>
+    <t>Atleast 2 ovservations per point</t>
+  </si>
+  <si>
+    <t>tape = c(0.5 - 50) by 0.5</t>
   </si>
 </sst>
 </file>
@@ -813,7 +842,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -832,6 +861,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,6 +877,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2323,10 +2357,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81344756-8421-4003-BB16-25DFCF8D1503}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2546,7 +2580,7 @@
         <v>7</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2554,7 +2588,7 @@
         <v>8</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2562,7 +2596,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2679,86 +2713,94 @@
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
-        <v>216</v>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>1</v>
-      </c>
-      <c r="B55" t="s">
-        <v>167</v>
+      <c r="A55" s="12" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B62" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
+        <v>8</v>
+      </c>
+      <c r="B63" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>9</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B64" s="18" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2781,7 +2823,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2805,7 +2847,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2813,7 +2855,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2821,7 +2863,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2869,7 +2911,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2906,7 +2948,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2914,7 +2956,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2922,7 +2964,7 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2930,7 +2972,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2967,7 +3009,7 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2975,7 +3017,7 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2991,7 +3033,7 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2999,7 +3041,7 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3007,7 +3049,7 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3028,7 +3070,7 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -3036,7 +3078,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -3052,7 +3094,7 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -3081,7 +3123,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -3105,7 +3147,7 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3113,7 +3155,7 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -3121,7 +3163,7 @@
         <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -3153,12 +3195,12 @@
         <v>9</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3170,8 +3212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1814C7-AA32-4067-9313-102B115335D4}">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3181,7 +3223,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -3205,7 +3247,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3213,7 +3255,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3221,7 +3263,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3229,7 +3271,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3261,7 +3303,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -3269,7 +3311,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -3306,7 +3348,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -3314,7 +3356,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -3322,7 +3364,7 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -3330,7 +3372,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -3375,7 +3417,7 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -3391,7 +3433,7 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -3399,7 +3441,7 @@
         <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3407,7 +3449,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3428,7 +3470,7 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -3436,7 +3478,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -3444,7 +3486,7 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -3473,7 +3515,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3489,7 +3531,7 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -3497,7 +3539,7 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -3505,7 +3547,7 @@
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3513,7 +3555,7 @@
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -3521,7 +3563,7 @@
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -3529,12 +3571,12 @@
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -3558,7 +3600,7 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -3574,7 +3616,7 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -3606,7 +3648,7 @@
         <v>9</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>201</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -3615,6 +3657,533 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2799E56D-53B1-4BC9-A9D8-0F2A4E8D2B2A}">
+  <dimension ref="A1:B64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="69.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>9</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>4</v>
+      </c>
+      <c r="B50" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>7</v>
+      </c>
+      <c r="B53" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2</v>
+      </c>
+      <c r="B57" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>4</v>
+      </c>
+      <c r="B59" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>6</v>
+      </c>
+      <c r="B61" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>8</v>
+      </c>
+      <c r="B63" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>9</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE21BC4-FC9D-4D48-82B6-2328DB4FC4F5}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FECDF020-F414-44C9-AC01-E2FBDD0C0A6F}">
   <dimension ref="A1:B34"/>
   <sheetViews>
@@ -3843,7 +4412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773B8C9A-01A4-466F-AF7F-C3E224991309}">
   <dimension ref="A1:B32"/>
   <sheetViews>

</xml_diff>